<commit_message>
Updated API Listing to be consistent with the DB
</commit_message>
<xml_diff>
--- a/documentations/API_specs_Charting.xlsx
+++ b/documentations/API_specs_Charting.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11010"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/akshaymutha/Desktop/NJIT_Courses_material/CS_673_Soft_Prod_meth_Vaish_Prabhat/Project_work/charting/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rahul\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84244429-B797-1F49-BDA6-CDE7D47347B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0090AC96-F466-436C-98E7-3AE854BB8F3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1360" yWindow="2380" windowWidth="28040" windowHeight="17340" xr2:uid="{38CCAD5E-4D3C-BB46-A3DC-602C2690E922}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{38CCAD5E-4D3C-BB46-A3DC-602C2690E922}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -23,9 +23,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
@@ -34,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="28">
   <si>
     <t>API Design &amp; Specifications (Charting team)</t>
   </si>
@@ -71,18 +69,6 @@
   </si>
   <si>
     <t>Documents</t>
-  </si>
-  <si>
-    <t>practicemgmtportal.com/doctor-info/get?doc_id=</t>
-  </si>
-  <si>
-    <t>practicemgmtportal.com/lab_reports/get?patient_id=</t>
-  </si>
-  <si>
-    <t>practicemgmtportal.com/medication-info/get?patient_id=</t>
-  </si>
-  <si>
-    <t>practicemgmtportal.com/documents/get?patient_id=</t>
   </si>
   <si>
     <t>{
@@ -138,6 +124,24 @@
   <si>
     <t>Documents contain the progress notes written by the doctors themselves which can be shared with patients as well.
 This data can be fetched from the database using patient id only.</t>
+  </si>
+  <si>
+    <t>practicemgmtportal.com/doctor-info/get?doctor_id={1}</t>
+  </si>
+  <si>
+    <t>practicemgmtportal.com/lab_reports/get?patient_id={1}&amp;doctor_id={2}&amp;lab_id={3}</t>
+  </si>
+  <si>
+    <t>practicemgmtportal.com/medication-info/get?patient_id={1}&amp;doctor_id={2}&amp;med_id={3}</t>
+  </si>
+  <si>
+    <t>practicemgmtportal.com/documents/get?patient_id={1}&amp;doctor_id={2}&amp;doc_id={3}</t>
+  </si>
+  <si>
+    <t>{1},{2},{3} … {i}</t>
+  </si>
+  <si>
+    <t>substitute_value here…</t>
   </si>
 </sst>
 </file>
@@ -190,14 +194,14 @@
   <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -516,24 +520,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43364C13-0924-4143-91AC-3CFB271055CF}">
-  <dimension ref="A1:I11"/>
+  <dimension ref="A1:I14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.83203125" customWidth="1"/>
+    <col min="1" max="1" width="24.796875" customWidth="1"/>
     <col min="2" max="2" width="18" customWidth="1"/>
-    <col min="3" max="3" width="49.6640625" customWidth="1"/>
+    <col min="3" max="3" width="76.296875" customWidth="1"/>
     <col min="4" max="4" width="20.5" customWidth="1"/>
-    <col min="5" max="5" width="25.33203125" customWidth="1"/>
+    <col min="5" max="5" width="25.296875" customWidth="1"/>
     <col min="6" max="6" width="44" customWidth="1"/>
     <col min="7" max="7" width="23" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" ht="21" x14ac:dyDescent="0.4">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -546,52 +550,52 @@
       <c r="H1" s="5"/>
       <c r="I1" s="5"/>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A2" s="1"/>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1"/>
-    </row>
-    <row r="3" spans="1:9" ht="40" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A2" s="4"/>
+      <c r="B2" s="4"/>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4"/>
+      <c r="H2" s="4"/>
+      <c r="I2" s="4"/>
+    </row>
+    <row r="3" spans="1:9" ht="36" x14ac:dyDescent="0.35">
+      <c r="A3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="E3" s="3" t="s">
+      <c r="D3" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="F3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G3" s="4" t="s">
+      <c r="G3" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A4" s="1"/>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
-      <c r="H4" s="1"/>
-      <c r="I4" s="1"/>
-    </row>
-    <row r="5" spans="1:9" ht="85" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A4" s="4"/>
+      <c r="B4" s="4"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="4"/>
+      <c r="H4" s="4"/>
+      <c r="I4" s="4"/>
+    </row>
+    <row r="5" spans="1:9" ht="78" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -599,31 +603,31 @@
         <v>8</v>
       </c>
       <c r="C5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2" t="s">
+      <c r="F5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G5" t="s">
         <v>16</v>
       </c>
-      <c r="F5" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="G5" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A6" s="1"/>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
-      <c r="G6" s="1"/>
-      <c r="H6" s="1"/>
-      <c r="I6" s="1"/>
-    </row>
-    <row r="7" spans="1:9" ht="153" x14ac:dyDescent="0.2">
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A6" s="4"/>
+      <c r="B6" s="4"/>
+      <c r="C6" s="4"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="4"/>
+      <c r="G6" s="4"/>
+      <c r="H6" s="4"/>
+      <c r="I6" s="4"/>
+    </row>
+    <row r="7" spans="1:9" ht="140.4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>9</v>
       </c>
@@ -631,30 +635,30 @@
         <v>8</v>
       </c>
       <c r="C7" t="s">
-        <v>13</v>
-      </c>
-      <c r="E7" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F7" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="F7" s="2" t="s">
-        <v>22</v>
-      </c>
       <c r="G7" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A8" s="1"/>
-      <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
-      <c r="G8" s="1"/>
-      <c r="H8" s="1"/>
-      <c r="I8" s="1"/>
-    </row>
-    <row r="9" spans="1:9" ht="119" x14ac:dyDescent="0.2">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A8" s="4"/>
+      <c r="B8" s="4"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="4"/>
+      <c r="G8" s="4"/>
+      <c r="H8" s="4"/>
+      <c r="I8" s="4"/>
+    </row>
+    <row r="9" spans="1:9" ht="109.2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -662,30 +666,30 @@
         <v>8</v>
       </c>
       <c r="C9" t="s">
-        <v>14</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="F9" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>19</v>
       </c>
       <c r="G9" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A10" s="1"/>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
-      <c r="G10" s="1"/>
-      <c r="H10" s="1"/>
-      <c r="I10" s="1"/>
-    </row>
-    <row r="11" spans="1:9" ht="102" x14ac:dyDescent="0.2">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A10" s="4"/>
+      <c r="B10" s="4"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4"/>
+      <c r="F10" s="4"/>
+      <c r="G10" s="4"/>
+      <c r="H10" s="4"/>
+      <c r="I10" s="4"/>
+    </row>
+    <row r="11" spans="1:9" ht="93.6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>11</v>
       </c>
@@ -693,16 +697,24 @@
         <v>8</v>
       </c>
       <c r="C11" t="s">
+        <v>25</v>
+      </c>
+      <c r="E11" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E11" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>25</v>
+      <c r="F11" s="1" t="s">
+        <v>21</v>
       </c>
       <c r="G11" t="s">
-        <v>20</v>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>27</v>
+      </c>
+      <c r="B14" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>